<commit_message>
austragung inventar ausleihe dig
</commit_message>
<xml_diff>
--- a/data/christoph/Intvent_final_0.2_cb.xlsx
+++ b/data/christoph/Intvent_final_0.2_cb.xlsx
@@ -20836,7 +20836,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -21174,6 +21174,11 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -21184,10 +21189,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -21524,8 +21527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A628" workbookViewId="0">
-      <selection activeCell="B660" sqref="B660"/>
+    <sheetView tabSelected="1" topLeftCell="A572" workbookViewId="0">
+      <selection activeCell="C593" sqref="C593"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -21621,11 +21624,11 @@
       <c r="E3" s="12" t="s">
         <v>2297</v>
       </c>
-      <c r="J3" s="135" t="s">
+      <c r="J3" s="138" t="s">
         <v>3929</v>
       </c>
-      <c r="K3" s="135"/>
-      <c r="L3" s="135"/>
+      <c r="K3" s="138"/>
+      <c r="L3" s="138"/>
       <c r="M3">
         <v>88</v>
       </c>
@@ -21734,10 +21737,10 @@
       <c r="I7" s="4" t="s">
         <v>2361</v>
       </c>
-      <c r="J7" s="135" t="s">
+      <c r="J7" s="138" t="s">
         <v>3964</v>
       </c>
-      <c r="K7" s="135"/>
+      <c r="K7" s="138"/>
       <c r="M7">
         <v>1</v>
       </c>
@@ -21796,11 +21799,11 @@
       <c r="I9" s="4" t="s">
         <v>2361</v>
       </c>
-      <c r="J9" s="135" t="s">
+      <c r="J9" s="138" t="s">
         <v>3921</v>
       </c>
-      <c r="K9" s="135"/>
-      <c r="L9" s="135"/>
+      <c r="K9" s="138"/>
+      <c r="L9" s="138"/>
       <c r="M9">
         <v>45</v>
       </c>
@@ -21906,11 +21909,11 @@
       <c r="H13" s="69" t="s">
         <v>3894</v>
       </c>
-      <c r="J13" s="135" t="s">
+      <c r="J13" s="138" t="s">
         <v>3917</v>
       </c>
-      <c r="K13" s="135"/>
-      <c r="L13" s="135"/>
+      <c r="K13" s="138"/>
+      <c r="L13" s="138"/>
       <c r="M13" s="12">
         <v>40</v>
       </c>
@@ -21933,12 +21936,12 @@
         <v>2170</v>
       </c>
       <c r="F14" s="12"/>
-      <c r="J14" s="135" t="s">
+      <c r="J14" s="138" t="s">
         <v>3847</v>
       </c>
-      <c r="K14" s="135"/>
-      <c r="L14" s="135"/>
-      <c r="M14" s="135"/>
+      <c r="K14" s="138"/>
+      <c r="L14" s="138"/>
+      <c r="M14" s="138"/>
       <c r="N14" s="12"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
@@ -22012,10 +22015,10 @@
         <v>2589</v>
       </c>
       <c r="F17" s="12"/>
-      <c r="J17" s="135" t="s">
+      <c r="J17" s="138" t="s">
         <v>3923</v>
       </c>
-      <c r="K17" s="135"/>
+      <c r="K17" s="138"/>
       <c r="M17" s="12">
         <v>83</v>
       </c>
@@ -22067,11 +22070,11 @@
         <v>2373</v>
       </c>
       <c r="F19" s="12"/>
-      <c r="J19" s="135" t="s">
+      <c r="J19" s="138" t="s">
         <v>2069</v>
       </c>
-      <c r="K19" s="135"/>
-      <c r="L19" s="135"/>
+      <c r="K19" s="138"/>
+      <c r="L19" s="138"/>
       <c r="M19" s="12">
         <v>10</v>
       </c>
@@ -22173,11 +22176,11 @@
         <v>2373</v>
       </c>
       <c r="F23" s="12"/>
-      <c r="J23" s="135" t="s">
+      <c r="J23" s="138" t="s">
         <v>2367</v>
       </c>
-      <c r="K23" s="135"/>
-      <c r="L23" s="135"/>
+      <c r="K23" s="138"/>
+      <c r="L23" s="138"/>
       <c r="M23" s="12">
         <v>60</v>
       </c>
@@ -22200,15 +22203,15 @@
         <v>2589</v>
       </c>
       <c r="F24" s="12"/>
-      <c r="H24" s="136" t="s">
+      <c r="H24" s="139" t="s">
         <v>2371</v>
       </c>
-      <c r="I24" s="136"/>
-      <c r="J24" s="135" t="s">
+      <c r="I24" s="139"/>
+      <c r="J24" s="138" t="s">
         <v>3892</v>
       </c>
-      <c r="K24" s="135"/>
-      <c r="L24" s="135"/>
+      <c r="K24" s="138"/>
+      <c r="L24" s="138"/>
       <c r="M24" s="7">
         <v>51</v>
       </c>
@@ -22236,10 +22239,10 @@
         <v>1868</v>
       </c>
       <c r="I25" s="40"/>
-      <c r="J25" s="137" t="s">
+      <c r="J25" s="140" t="s">
         <v>4271</v>
       </c>
-      <c r="K25" s="137"/>
+      <c r="K25" s="140"/>
       <c r="L25" s="38"/>
       <c r="M25" s="39" t="s">
         <v>2244</v>
@@ -22265,11 +22268,11 @@
         <v>2589</v>
       </c>
       <c r="F26" s="12"/>
-      <c r="J26" s="135" t="s">
+      <c r="J26" s="138" t="s">
         <v>948</v>
       </c>
-      <c r="K26" s="135"/>
-      <c r="L26" s="135"/>
+      <c r="K26" s="138"/>
+      <c r="L26" s="138"/>
       <c r="M26" s="7">
         <v>4</v>
       </c>
@@ -22322,11 +22325,11 @@
       <c r="H28" s="7">
         <v>1887</v>
       </c>
-      <c r="J28" s="135" t="s">
+      <c r="J28" s="138" t="s">
         <v>3893</v>
       </c>
-      <c r="K28" s="135"/>
-      <c r="L28" s="135"/>
+      <c r="K28" s="138"/>
+      <c r="L28" s="138"/>
       <c r="M28" s="7">
         <v>6</v>
       </c>
@@ -22355,10 +22358,10 @@
       <c r="H29" s="7">
         <v>1897</v>
       </c>
-      <c r="J29" s="135" t="s">
+      <c r="J29" s="138" t="s">
         <v>2539</v>
       </c>
-      <c r="K29" s="135"/>
+      <c r="K29" s="138"/>
       <c r="L29" s="12"/>
       <c r="M29" s="7">
         <v>2</v>
@@ -22445,11 +22448,11 @@
       <c r="H32" s="7">
         <v>1905</v>
       </c>
-      <c r="J32" s="135" t="s">
+      <c r="J32" s="138" t="s">
         <v>3956</v>
       </c>
-      <c r="K32" s="135"/>
-      <c r="L32" s="135"/>
+      <c r="K32" s="138"/>
+      <c r="L32" s="138"/>
       <c r="M32" s="7">
         <v>26</v>
       </c>
@@ -22475,11 +22478,11 @@
       <c r="H33" s="7">
         <v>1905</v>
       </c>
-      <c r="J33" s="135" t="s">
+      <c r="J33" s="138" t="s">
         <v>3957</v>
       </c>
-      <c r="K33" s="135"/>
-      <c r="L33" s="135"/>
+      <c r="K33" s="138"/>
+      <c r="L33" s="138"/>
       <c r="M33" s="7">
         <v>11</v>
       </c>
@@ -22535,11 +22538,11 @@
       <c r="H35" s="7">
         <v>1905</v>
       </c>
-      <c r="J35" s="135" t="s">
+      <c r="J35" s="138" t="s">
         <v>3821</v>
       </c>
-      <c r="K35" s="135"/>
-      <c r="L35" s="135"/>
+      <c r="K35" s="138"/>
+      <c r="L35" s="138"/>
       <c r="M35" s="7">
         <v>23</v>
       </c>
@@ -22601,10 +22604,10 @@
       <c r="I37" s="4" t="s">
         <v>2128</v>
       </c>
-      <c r="J37" s="135" t="s">
+      <c r="J37" s="138" t="s">
         <v>2015</v>
       </c>
-      <c r="K37" s="135"/>
+      <c r="K37" s="138"/>
       <c r="L37" s="12"/>
       <c r="M37" s="7">
         <v>11</v>
@@ -22631,11 +22634,11 @@
       <c r="I38" s="106" t="s">
         <v>2128</v>
       </c>
-      <c r="J38" s="135" t="s">
+      <c r="J38" s="138" t="s">
         <v>167</v>
       </c>
-      <c r="K38" s="135"/>
-      <c r="L38" s="135"/>
+      <c r="K38" s="138"/>
+      <c r="L38" s="138"/>
       <c r="M38" s="7">
         <v>8</v>
       </c>
@@ -22661,10 +22664,10 @@
       <c r="H39" s="7">
         <v>1898</v>
       </c>
-      <c r="J39" s="135" t="s">
+      <c r="J39" s="138" t="s">
         <v>3822</v>
       </c>
-      <c r="K39" s="135"/>
+      <c r="K39" s="138"/>
       <c r="M39" s="7">
         <v>7</v>
       </c>
@@ -22695,11 +22698,11 @@
       <c r="H40" s="7">
         <v>1898</v>
       </c>
-      <c r="J40" s="135" t="s">
+      <c r="J40" s="138" t="s">
         <v>3899</v>
       </c>
-      <c r="K40" s="135"/>
-      <c r="L40" s="135"/>
+      <c r="K40" s="138"/>
+      <c r="L40" s="138"/>
       <c r="M40" s="7">
         <v>33</v>
       </c>
@@ -22752,10 +22755,10 @@
         <v>2589</v>
       </c>
       <c r="F42" s="12"/>
-      <c r="J42" s="135" t="s">
+      <c r="J42" s="138" t="s">
         <v>3901</v>
       </c>
-      <c r="K42" s="135"/>
+      <c r="K42" s="138"/>
       <c r="L42" s="12"/>
       <c r="M42" s="7">
         <v>9</v>
@@ -22779,10 +22782,10 @@
         <v>2589</v>
       </c>
       <c r="F43" s="12"/>
-      <c r="J43" s="135" t="s">
+      <c r="J43" s="138" t="s">
         <v>2326</v>
       </c>
-      <c r="K43" s="135"/>
+      <c r="K43" s="138"/>
       <c r="L43" s="12"/>
       <c r="M43" s="7">
         <v>71</v>
@@ -22944,11 +22947,11 @@
         <v>2589</v>
       </c>
       <c r="F49" s="12"/>
-      <c r="J49" s="135" t="s">
+      <c r="J49" s="138" t="s">
         <v>2302</v>
       </c>
-      <c r="K49" s="135"/>
-      <c r="L49" s="135"/>
+      <c r="K49" s="138"/>
+      <c r="L49" s="138"/>
       <c r="M49" s="7">
         <v>2</v>
       </c>
@@ -22974,11 +22977,11 @@
       <c r="H50" s="7">
         <v>1898</v>
       </c>
-      <c r="J50" s="135" t="s">
+      <c r="J50" s="138" t="s">
         <v>3902</v>
       </c>
-      <c r="K50" s="135"/>
-      <c r="L50" s="135"/>
+      <c r="K50" s="138"/>
+      <c r="L50" s="138"/>
       <c r="M50" s="7">
         <v>19</v>
       </c>
@@ -23061,11 +23064,11 @@
       <c r="H53" s="7">
         <v>1903</v>
       </c>
-      <c r="J53" s="135" t="s">
+      <c r="J53" s="138" t="s">
         <v>3872</v>
       </c>
-      <c r="K53" s="135"/>
-      <c r="L53" s="135"/>
+      <c r="K53" s="138"/>
+      <c r="L53" s="138"/>
       <c r="M53" s="7">
         <v>12</v>
       </c>
@@ -23088,11 +23091,11 @@
         <v>2589</v>
       </c>
       <c r="F54" s="12"/>
-      <c r="J54" s="135" t="s">
+      <c r="J54" s="138" t="s">
         <v>3877</v>
       </c>
-      <c r="K54" s="135"/>
-      <c r="L54" s="135"/>
+      <c r="K54" s="138"/>
+      <c r="L54" s="138"/>
       <c r="M54" s="7">
         <v>49</v>
       </c>
@@ -23169,11 +23172,11 @@
         <v>2589</v>
       </c>
       <c r="F57" s="12"/>
-      <c r="J57" s="135" t="s">
+      <c r="J57" s="138" t="s">
         <v>2374</v>
       </c>
-      <c r="K57" s="135"/>
-      <c r="L57" s="135"/>
+      <c r="K57" s="138"/>
+      <c r="L57" s="138"/>
       <c r="M57" s="7">
         <v>7</v>
       </c>
@@ -23199,10 +23202,10 @@
       <c r="G58" s="69" t="s">
         <v>3931</v>
       </c>
-      <c r="J58" s="135" t="s">
+      <c r="J58" s="138" t="s">
         <v>3930</v>
       </c>
-      <c r="K58" s="135"/>
+      <c r="K58" s="138"/>
       <c r="M58" s="7">
         <v>11</v>
       </c>
@@ -23230,10 +23233,10 @@
       <c r="I59" s="106" t="s">
         <v>2128</v>
       </c>
-      <c r="J59" s="135" t="s">
+      <c r="J59" s="138" t="s">
         <v>3932</v>
       </c>
-      <c r="K59" s="135"/>
+      <c r="K59" s="138"/>
       <c r="M59" s="7">
         <v>20</v>
       </c>
@@ -23264,11 +23267,11 @@
       <c r="I60" s="106" t="s">
         <v>2128</v>
       </c>
-      <c r="J60" s="135" t="s">
+      <c r="J60" s="138" t="s">
         <v>3854</v>
       </c>
-      <c r="K60" s="135"/>
-      <c r="L60" s="135"/>
+      <c r="K60" s="138"/>
+      <c r="L60" s="138"/>
       <c r="M60" s="7">
         <v>10</v>
       </c>
@@ -23417,11 +23420,11 @@
         <v>2589</v>
       </c>
       <c r="F65" s="12"/>
-      <c r="J65" s="135" t="s">
+      <c r="J65" s="138" t="s">
         <v>2073</v>
       </c>
-      <c r="K65" s="135"/>
-      <c r="L65" s="135"/>
+      <c r="K65" s="138"/>
+      <c r="L65" s="138"/>
       <c r="M65" s="7">
         <v>13</v>
       </c>
@@ -23477,10 +23480,10 @@
       <c r="I67" s="106" t="s">
         <v>2128</v>
       </c>
-      <c r="J67" s="135" t="s">
+      <c r="J67" s="138" t="s">
         <v>3906</v>
       </c>
-      <c r="K67" s="135"/>
+      <c r="K67" s="138"/>
       <c r="M67" s="7">
         <v>12</v>
       </c>
@@ -23514,11 +23517,11 @@
       <c r="I68" s="4" t="s">
         <v>2128</v>
       </c>
-      <c r="J68" s="135" t="s">
+      <c r="J68" s="138" t="s">
         <v>303</v>
       </c>
-      <c r="K68" s="135"/>
-      <c r="L68" s="135"/>
+      <c r="K68" s="138"/>
+      <c r="L68" s="138"/>
       <c r="M68" s="7">
         <v>38</v>
       </c>
@@ -23541,10 +23544,10 @@
         <v>2589</v>
       </c>
       <c r="F69" s="12"/>
-      <c r="J69" s="135" t="s">
+      <c r="J69" s="138" t="s">
         <v>3926</v>
       </c>
-      <c r="K69" s="135"/>
+      <c r="K69" s="138"/>
       <c r="L69" s="12"/>
       <c r="M69" s="7">
         <v>9</v>
@@ -23571,11 +23574,11 @@
       <c r="H70" s="69" t="s">
         <v>3927</v>
       </c>
-      <c r="J70" s="135" t="s">
+      <c r="J70" s="138" t="s">
         <v>3949</v>
       </c>
-      <c r="K70" s="135"/>
-      <c r="L70" s="135"/>
+      <c r="K70" s="138"/>
+      <c r="L70" s="138"/>
       <c r="M70" s="7">
         <v>22</v>
       </c>
@@ -23625,10 +23628,10 @@
         <v>2589</v>
       </c>
       <c r="F72" s="12"/>
-      <c r="J72" s="135" t="s">
+      <c r="J72" s="138" t="s">
         <v>3992</v>
       </c>
-      <c r="K72" s="135"/>
+      <c r="K72" s="138"/>
       <c r="L72" s="12"/>
       <c r="M72" s="7">
         <v>6</v>
@@ -23715,11 +23718,11 @@
       <c r="H75" s="69" t="s">
         <v>3976</v>
       </c>
-      <c r="J75" s="135" t="s">
+      <c r="J75" s="138" t="s">
         <v>3982</v>
       </c>
-      <c r="K75" s="135"/>
-      <c r="L75" s="135"/>
+      <c r="K75" s="138"/>
+      <c r="L75" s="138"/>
       <c r="M75" s="7">
         <v>10</v>
       </c>
@@ -23775,10 +23778,10 @@
       <c r="I77" s="106" t="s">
         <v>2128</v>
       </c>
-      <c r="J77" s="135" t="s">
+      <c r="J77" s="138" t="s">
         <v>3983</v>
       </c>
-      <c r="K77" s="135"/>
+      <c r="K77" s="138"/>
       <c r="L77" s="12"/>
       <c r="M77" s="7">
         <v>4</v>
@@ -23829,11 +23832,11 @@
         <v>2156</v>
       </c>
       <c r="F79" s="12"/>
-      <c r="J79" s="135" t="s">
+      <c r="J79" s="138" t="s">
         <v>3945</v>
       </c>
-      <c r="K79" s="135"/>
-      <c r="L79" s="135"/>
+      <c r="K79" s="138"/>
+      <c r="L79" s="138"/>
       <c r="M79" s="7">
         <v>1</v>
       </c>
@@ -23856,11 +23859,11 @@
         <v>2156</v>
       </c>
       <c r="F80" s="12"/>
-      <c r="J80" s="135" t="s">
+      <c r="J80" s="138" t="s">
         <v>2497</v>
       </c>
-      <c r="K80" s="135"/>
-      <c r="L80" s="135"/>
+      <c r="K80" s="138"/>
+      <c r="L80" s="138"/>
       <c r="M80" s="7">
         <v>2</v>
       </c>
@@ -23883,11 +23886,11 @@
         <v>2156</v>
       </c>
       <c r="F81" s="12"/>
-      <c r="J81" s="135" t="s">
+      <c r="J81" s="138" t="s">
         <v>3977</v>
       </c>
-      <c r="K81" s="135"/>
-      <c r="L81" s="135"/>
+      <c r="K81" s="138"/>
+      <c r="L81" s="138"/>
       <c r="M81" s="7">
         <v>3</v>
       </c>
@@ -23910,10 +23913,10 @@
         <v>2156</v>
       </c>
       <c r="F82" s="12"/>
-      <c r="J82" s="135" t="s">
+      <c r="J82" s="138" t="s">
         <v>2489</v>
       </c>
-      <c r="K82" s="135"/>
+      <c r="K82" s="138"/>
       <c r="L82" s="12"/>
       <c r="M82" s="7">
         <v>1</v>
@@ -24019,11 +24022,11 @@
       <c r="H86" s="7" t="s">
         <v>2267</v>
       </c>
-      <c r="J86" s="135" t="s">
+      <c r="J86" s="138" t="s">
         <v>3979</v>
       </c>
-      <c r="K86" s="135"/>
-      <c r="L86" s="135"/>
+      <c r="K86" s="138"/>
+      <c r="L86" s="138"/>
       <c r="M86" s="7">
         <v>8</v>
       </c>
@@ -33597,7 +33600,7 @@
       <c r="A410" s="4">
         <v>0</v>
       </c>
-      <c r="B410" s="85" t="s">
+      <c r="B410" s="13" t="s">
         <v>2936</v>
       </c>
       <c r="C410" s="38" t="s">
@@ -33616,7 +33619,7 @@
       <c r="H410" s="39">
         <v>1890</v>
       </c>
-      <c r="I410" s="107" t="s">
+      <c r="I410" s="141" t="s">
         <v>4786</v>
       </c>
       <c r="J410" s="118" t="s">
@@ -34310,7 +34313,7 @@
       <c r="A429" s="4">
         <v>0</v>
       </c>
-      <c r="B429" s="85" t="s">
+      <c r="B429" s="13" t="s">
         <v>3098</v>
       </c>
       <c r="C429" s="13" t="s">
@@ -40665,7 +40668,7 @@
       <c r="A624" s="4">
         <v>0</v>
       </c>
-      <c r="B624" s="139" t="s">
+      <c r="B624" s="136" t="s">
         <v>2736</v>
       </c>
       <c r="C624" s="13" t="s">
@@ -40803,7 +40806,7 @@
       <c r="A628" s="4">
         <v>0</v>
       </c>
-      <c r="B628" s="139" t="s">
+      <c r="B628" s="136" t="s">
         <v>3001</v>
       </c>
       <c r="C628" s="13" t="s">
@@ -40821,7 +40824,7 @@
         <v>3003</v>
       </c>
       <c r="I628" s="14"/>
-      <c r="J628" s="138" t="s">
+      <c r="J628" s="135" t="s">
         <v>4955</v>
       </c>
       <c r="K628" s="13"/>
@@ -40837,7 +40840,7 @@
       <c r="A629" s="4">
         <v>0</v>
       </c>
-      <c r="B629" s="139" t="s">
+      <c r="B629" s="136" t="s">
         <v>3236</v>
       </c>
       <c r="C629" s="13" t="s">
@@ -41434,7 +41437,7 @@
       <c r="A648" s="4">
         <v>0</v>
       </c>
-      <c r="B648" s="139" t="s">
+      <c r="B648" s="136" t="s">
         <v>3029</v>
       </c>
       <c r="C648" s="18" t="s">
@@ -41798,7 +41801,7 @@
       <c r="A660" s="4">
         <v>0</v>
       </c>
-      <c r="B660" s="139" t="s">
+      <c r="B660" s="136" t="s">
         <v>3288</v>
       </c>
       <c r="C660" s="13" t="s">
@@ -41938,7 +41941,7 @@
       <c r="A664" s="4">
         <v>0</v>
       </c>
-      <c r="B664" s="139" t="s">
+      <c r="B664" s="136" t="s">
         <v>2799</v>
       </c>
       <c r="C664" s="13" t="s">
@@ -42076,7 +42079,7 @@
       <c r="A668" s="4">
         <v>0</v>
       </c>
-      <c r="B668" s="139" t="s">
+      <c r="B668" s="136" t="s">
         <v>2789</v>
       </c>
       <c r="C668" s="38" t="s">
@@ -42327,7 +42330,7 @@
       <c r="A676" s="4">
         <v>0</v>
       </c>
-      <c r="B676" s="139" t="s">
+      <c r="B676" s="136" t="s">
         <v>3387</v>
       </c>
       <c r="C676" s="18" t="s">
@@ -42417,7 +42420,7 @@
       <c r="A679" s="4">
         <v>0</v>
       </c>
-      <c r="B679" s="139" t="s">
+      <c r="B679" s="136" t="s">
         <v>3339</v>
       </c>
       <c r="C679" s="18" t="s">
@@ -42446,7 +42449,7 @@
       <c r="A680" s="4">
         <v>0</v>
       </c>
-      <c r="B680" s="139" t="s">
+      <c r="B680" s="136" t="s">
         <v>3340</v>
       </c>
       <c r="C680" s="18" t="s">
@@ -42475,7 +42478,7 @@
       <c r="A681" s="4">
         <v>0</v>
       </c>
-      <c r="B681" s="139" t="s">
+      <c r="B681" s="136" t="s">
         <v>3131</v>
       </c>
       <c r="C681" s="18" t="s">
@@ -42501,7 +42504,7 @@
       <c r="A682" s="4">
         <v>0</v>
       </c>
-      <c r="B682" s="139" t="s">
+      <c r="B682" s="136" t="s">
         <v>3023</v>
       </c>
       <c r="C682" s="18" t="s">
@@ -42533,7 +42536,7 @@
       <c r="A683" s="4">
         <v>0</v>
       </c>
-      <c r="B683" s="139" t="s">
+      <c r="B683" s="136" t="s">
         <v>3182</v>
       </c>
       <c r="C683" s="18" t="s">
@@ -42559,7 +42562,7 @@
       <c r="A684" s="4">
         <v>0</v>
       </c>
-      <c r="B684" s="139" t="s">
+      <c r="B684" s="136" t="s">
         <v>3443</v>
       </c>
       <c r="C684" s="18" t="s">
@@ -43003,7 +43006,7 @@
       <c r="A702" s="4">
         <v>0</v>
       </c>
-      <c r="B702" s="140"/>
+      <c r="B702" s="137"/>
       <c r="C702" s="18" t="s">
         <v>2977</v>
       </c>
@@ -43852,7 +43855,7 @@
       <c r="A728" s="4">
         <v>0</v>
       </c>
-      <c r="B728" s="139" t="s">
+      <c r="B728" s="136" t="s">
         <v>1529</v>
       </c>
       <c r="C728" s="18" t="s">
@@ -60349,26 +60352,16 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="J68:L68"/>
-    <mergeCell ref="J69:K69"/>
-    <mergeCell ref="J86:L86"/>
-    <mergeCell ref="J77:K77"/>
-    <mergeCell ref="J79:L79"/>
-    <mergeCell ref="J80:L80"/>
-    <mergeCell ref="J81:L81"/>
-    <mergeCell ref="J82:K82"/>
-    <mergeCell ref="J75:L75"/>
-    <mergeCell ref="J70:L70"/>
-    <mergeCell ref="J72:K72"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="J35:L35"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J26:L26"/>
-    <mergeCell ref="J32:L32"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J19:L19"/>
     <mergeCell ref="J59:K59"/>
     <mergeCell ref="J60:L60"/>
     <mergeCell ref="J65:L65"/>
@@ -60383,16 +60376,26 @@
     <mergeCell ref="J54:L54"/>
     <mergeCell ref="J57:L57"/>
     <mergeCell ref="J58:K58"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="J35:L35"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="J32:L32"/>
+    <mergeCell ref="J68:L68"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="J86:L86"/>
+    <mergeCell ref="J77:K77"/>
+    <mergeCell ref="J79:L79"/>
+    <mergeCell ref="J80:L80"/>
+    <mergeCell ref="J81:L81"/>
+    <mergeCell ref="J82:K82"/>
+    <mergeCell ref="J75:L75"/>
+    <mergeCell ref="J70:L70"/>
+    <mergeCell ref="J72:K72"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>